<commit_message>
Implement access to cells via symbolic references
Considering sparse tables, column elements in sheet's XML are not always
accessible by direct indexing on their parent row element. Therefore the
only reliable way to locate a cell is by looking it up with "A1"-style
reference:

    my $cells = $sheet.workbook.worksheets[0].cells;
    say $cells["A1"];
    say $cells[1;"A"];
    $cells["ABZ255"]:exists;
    $cells[255;"ABZ"]:exists;
    $cells["BC42"] = $cell;
</commit_message>
<xml_diff>
--- a/t/test-data/stylish.xlsx
+++ b/t/test-data/stylish.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vrurg/src/Raku/spreadsheet-xlsx/t/test-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C076A8-2C46-DC45-B2C6-B0717E6477D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E2658BF-E33A-594D-9832-A9A0A7566016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28980" yWindow="2140" windowWidth="31900" windowHeight="23780" xr2:uid="{684AC051-B414-E348-986B-1FE37ABFDA0D}"/>
   </bookViews>
@@ -33,12 +33,65 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Foo</t>
   </si>
   <si>
     <t>Fubarish</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Bold</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Italic</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>Font</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -49,7 +102,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -69,6 +122,28 @@
       <color theme="1"/>
       <name val="Lucida Sans"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -495,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9D1EFC8-6FAA-D549-B76B-66DCB7D962C9}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -536,6 +611,11 @@
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
     </row>
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix a couple of bugs and tests
</commit_message>
<xml_diff>
--- a/t/test-data/stylish.xlsx
+++ b/t/test-data/stylish.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vrurg/src/Raku/spreadsheet-xlsx/t/test-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E2658BF-E33A-594D-9832-A9A0A7566016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC40A5F-9453-5C4E-80D1-61B0C5620985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28980" yWindow="2140" windowWidth="31900" windowHeight="23780" xr2:uid="{684AC051-B414-E348-986B-1FE37ABFDA0D}"/>
+    <workbookView xWindow="25280" yWindow="3080" windowWidth="31900" windowHeight="23780" xr2:uid="{684AC051-B414-E348-986B-1FE37ABFDA0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -98,9 +98,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
+    <numFmt numFmtId="166" formatCode="\₴#,###"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -238,7 +239,7 @@
       <alignment vertical="center" textRotation="12"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -250,6 +251,7 @@
       <alignment vertical="center" textRotation="12"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Fubar" xfId="1" xr:uid="{E7CB65CD-6E50-9B47-90AD-0E3F17F2428E}"/>
@@ -573,7 +575,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -607,7 +609,9 @@
       <c r="A4" s="8">
         <v>123.45677999999999</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="9">
+        <v>7890.1234560000003</v>
+      </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
     </row>

</xml_diff>